<commit_message>
Small update to $U
</commit_message>
<xml_diff>
--- a/$U.xlsx
+++ b/$U.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E1E956-276C-402A-9EB9-8222DFCE87A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF93120-3B5F-4D9B-A818-7E7CBB5A8307}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{F269EFF2-FA4C-41FB-BF44-2323E10B64BA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="99">
   <si>
     <t>$U</t>
   </si>
@@ -311,17 +311,30 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Book Value</t>
+  </si>
+  <si>
+    <t>Book Value per Share</t>
+  </si>
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>P/B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,7 +393,20 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -506,7 +532,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -540,9 +566,12 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -552,10 +581,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -574,8 +599,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -997,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2628023B-8E8D-4DD9-8B67-9E53DD821B70}">
-  <dimension ref="B2:I18"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="C22" sqref="C22:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1019,30 +1058,30 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
-      <c r="G5" s="24" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
+      <c r="G5" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="26"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4">
-        <v>37.54</v>
+        <v>28.8</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
@@ -1054,11 +1093,11 @@
       <c r="D7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
@@ -1066,14 +1105,14 @@
       </c>
       <c r="C8" s="8">
         <f>C6*C7</f>
-        <v>11112.328132620001</v>
+        <v>8525.1744864000011</v>
       </c>
       <c r="D8" s="15"/>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
@@ -1086,11 +1125,11 @@
       <c r="D9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="29"/>
-      <c r="I9" s="30"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
@@ -1122,68 +1161,81 @@
       </c>
       <c r="C12" s="9">
         <f>C8-C11</f>
-        <v>11638.138132620001</v>
+        <v>9050.9844864000006</v>
       </c>
       <c r="D12" s="7"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="G15" s="24" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
+      <c r="G15" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="G16" s="31" t="s">
+      <c r="D16" s="25"/>
+      <c r="G16" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="G17" s="31" t="s">
+      <c r="D17" s="25"/>
+      <c r="G17" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="11"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="30"/>
-      <c r="G18" s="34" t="s">
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="G18" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="37"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="43">
+        <f>C6/'Financial Model'!H59</f>
+        <v>3.5887007639676196</v>
+      </c>
+      <c r="D22" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:I5"/>
+  <mergeCells count="16">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
@@ -1192,6 +1244,12 @@
     <mergeCell ref="G16:I16"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="259" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
@@ -1200,28 +1258,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B1C713-6FB6-42FB-B1D6-8C35788D1E1A}">
-  <dimension ref="A1:AB56"/>
+  <dimension ref="A1:AB59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomRight" activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="16"/>
       <c r="D1" s="17" t="s">
@@ -1294,16 +1352,17 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="23" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="D2" s="23" t="s">
+    <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="D2" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="40" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20"/>
       <c r="B3" s="2" t="s">
         <v>24</v>
@@ -1315,7 +1374,7 @@
         <v>320.12599999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1326,7 +1385,7 @@
         <v>93.832999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>26</v>
@@ -1340,7 +1399,7 @@
         <v>226.29299999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1351,7 +1410,7 @@
         <v>221.04</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1362,7 +1421,7 @@
         <v>103.93899999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1373,7 +1432,7 @@
         <v>72.474999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1386,7 +1445,7 @@
         <v>397.45399999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:28" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>31</v>
@@ -1400,7 +1459,7 @@
         <v>-171.16099999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1411,7 +1470,7 @@
         <v>1.111</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1422,7 +1481,7 @@
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
         <v>34</v>
@@ -1436,7 +1495,7 @@
         <v>-171.33099999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1447,7 +1506,7 @@
         <v>6.2240000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>37</v>
@@ -1461,7 +1520,7 @@
         <v>-177.55499999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
@@ -1474,7 +1533,7 @@
         <v>-0.60322890796728945</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1488,7 +1547,7 @@
         <v>294.34100000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1501,7 +1560,7 @@
         <v>0.70688728813029866</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1514,7 +1573,7 @@
         <v>-0.53466759963264465</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1527,7 +1586,7 @@
         <v>-0.55464098511211202</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>41</v>
       </c>
@@ -1540,7 +1599,7 @@
         <v>1.9442344576822878E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1549,23 +1608,23 @@
         <v>0.36356124239687859</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K26" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="1" t="s">
         <v>6</v>
@@ -1574,7 +1633,7 @@
         <v>1152.0139999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>60</v>
@@ -1583,7 +1642,7 @@
         <v>656.58100000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>61</v>
@@ -1592,7 +1651,7 @@
         <v>332.95800000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>62</v>
@@ -1601,7 +1660,7 @@
         <v>48.734000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
@@ -1609,7 +1668,7 @@
         <v>33.909999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>64</v>
       </c>
@@ -1618,7 +1677,7 @@
         <v>2224.1969999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>84</v>
       </c>
@@ -1626,7 +1685,7 @@
         <v>110.17</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="1" t="s">
         <v>65</v>
@@ -1635,7 +1694,7 @@
         <v>101.486</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>66</v>
       </c>
@@ -1644,7 +1703,7 @@
         <v>2446.9610000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>67</v>
       </c>
@@ -1652,7 +1711,7 @@
         <v>10.678000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>68</v>
       </c>
@@ -1660,7 +1719,7 @@
         <v>53.167999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>69</v>
       </c>
@@ -1669,10 +1728,10 @@
         <v>4946.66</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H41" s="20"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>70</v>
       </c>
@@ -1680,7 +1739,7 @@
         <v>13.005000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>71</v>
       </c>
@@ -1688,7 +1747,7 @@
         <v>121.976</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>72</v>
       </c>
@@ -1696,7 +1755,7 @@
         <v>213.857</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>35</v>
       </c>
@@ -1704,7 +1763,7 @@
         <v>54.74</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>73</v>
       </c>
@@ -1712,7 +1771,7 @@
         <v>200.21799999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>74</v>
       </c>
@@ -1720,7 +1779,7 @@
         <v>26.463999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>75</v>
       </c>
@@ -1729,7 +1788,7 @@
         <v>630.26</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>76</v>
       </c>
@@ -1737,7 +1796,7 @@
         <v>1704.145</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>77</v>
       </c>
@@ -1745,7 +1804,7 @@
         <v>145.67599999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>78</v>
       </c>
@@ -1753,7 +1812,7 @@
         <v>94.34</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>79</v>
       </c>
@@ -1761,7 +1820,7 @@
         <v>10.097</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="1" t="s">
         <v>80</v>
@@ -1771,10 +1830,10 @@
         <v>2584.518</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H54" s="20"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>81</v>
       </c>
@@ -1782,13 +1841,31 @@
         <v>2362.1419999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
         <v>82</v>
       </c>
       <c r="H56" s="20">
         <f>H55+H53</f>
         <v>4946.66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H58" s="20">
+        <f>H40-H53</f>
+        <v>2362.1419999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H59" s="1">
+        <f>H58/H17</f>
+        <v>8.0251884718744577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>